<commit_message>
updated the requirements list
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t>Requirement #</t>
   </si>
@@ -91,13 +91,127 @@
   </si>
   <si>
     <t>9a</t>
+  </si>
+  <si>
+    <t>R-AC1</t>
+  </si>
+  <si>
+    <t>R-AC2</t>
+  </si>
+  <si>
+    <t>R-AC3</t>
+  </si>
+  <si>
+    <t>R-AC4</t>
+  </si>
+  <si>
+    <t>R-AC5</t>
+  </si>
+  <si>
+    <t>R-FA1</t>
+  </si>
+  <si>
+    <t>R-FA2</t>
+  </si>
+  <si>
+    <t>R-FA3</t>
+  </si>
+  <si>
+    <t>R-FA4</t>
+  </si>
+  <si>
+    <t>R-FA5</t>
+  </si>
+  <si>
+    <t>R-FA6</t>
+  </si>
+  <si>
+    <t>R-FA7</t>
+  </si>
+  <si>
+    <t>R-FA8</t>
+  </si>
+  <si>
+    <t>R-AV1</t>
+  </si>
+  <si>
+    <t>R-AV2</t>
+  </si>
+  <si>
+    <t>R-AV3</t>
+  </si>
+  <si>
+    <t>R-PD8</t>
+  </si>
+  <si>
+    <t>R-PD9</t>
+  </si>
+  <si>
+    <t>R-PD1</t>
+  </si>
+  <si>
+    <t>R-PD2</t>
+  </si>
+  <si>
+    <t>R-PD3</t>
+  </si>
+  <si>
+    <t>R-PD4</t>
+  </si>
+  <si>
+    <t>R-PV1</t>
+  </si>
+  <si>
+    <t>R-PV2</t>
+  </si>
+  <si>
+    <t>R-PV3</t>
+  </si>
+  <si>
+    <t>R-PV4</t>
+  </si>
+  <si>
+    <t>R-PD6</t>
+  </si>
+  <si>
+    <t>R-PD7</t>
+  </si>
+  <si>
+    <t>R-PV7</t>
+  </si>
+  <si>
+    <t>R-UP1</t>
+  </si>
+  <si>
+    <t>R-UP2</t>
+  </si>
+  <si>
+    <t>R-A</t>
+  </si>
+  <si>
+    <t>R-B</t>
+  </si>
+  <si>
+    <t>R-C</t>
+  </si>
+  <si>
+    <t>R-D</t>
+  </si>
+  <si>
+    <t>R-E</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Requirement Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +223,27 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -144,6 +279,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,20 +579,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,269 +601,423 @@
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>18</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="B3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="B4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="3">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="3">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="B8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="3">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="B9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="B11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="3">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="3">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="B13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="3">
         <v>7</v>
       </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="B15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="B16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="3">
         <v>8</v>
       </c>
-      <c r="B17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="B17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="B18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="3">
         <v>9</v>
       </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="B19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="B20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="B21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="B22" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="3">
         <v>10</v>
       </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="B23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="B24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="B25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="B26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="3">
         <v>11</v>
       </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="B27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="B28" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="B29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="B30" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="B31" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="B32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="3">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="B33" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B34" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="4">
+      <c r="B34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="4">
         <v>40836</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="4">
+      <c r="B35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="4">
         <v>40836</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="3" t="s">
+      <c r="B37" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="3" t="s">
-        <v>20</v>
+      <c r="B38" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added deletion confirmation for photos and albums.
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="19155" windowHeight="8505"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -163,13 +163,19 @@
   </si>
   <si>
     <t>R-PR1</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>on remove album, removing last album and creating new one, recreates the new one and the one just removed. Check on close function for album</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +257,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -329,6 +340,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -363,6 +375,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -538,21 +551,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -562,16 +575,25 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>40843</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -579,7 +601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -587,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -595,7 +617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -603,15 +625,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -619,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -627,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -635,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -643,7 +668,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -651,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -659,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -667,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -675,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -683,7 +708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -691,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -699,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -707,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -715,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -723,7 +748,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -731,7 +756,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -739,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -747,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -755,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -763,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -771,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -779,7 +804,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -787,7 +812,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -795,7 +820,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -803,7 +828,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -811,7 +836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -819,7 +844,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -827,7 +852,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -835,7 +860,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -843,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -851,7 +876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -859,7 +884,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
@@ -870,7 +895,7 @@
         <v>40836</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
@@ -881,7 +906,7 @@
         <v>40836</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>37</v>
       </c>
@@ -889,7 +914,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>38</v>
       </c>
@@ -897,7 +922,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>39</v>
       </c>
@@ -908,7 +933,7 @@
         <v>40838</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>46</v>
       </c>
@@ -916,7 +941,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>48</v>
       </c>
@@ -931,24 +956,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
image rotation now works going cc & ccw. in form main i added a bunch of member variables that should allow for much easier file selectors.
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="19155" windowHeight="8505"/>
@@ -174,8 +174,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,7 +340,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -375,7 +374,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -551,21 +549,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -579,7 +577,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -593,7 +591,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -601,7 +599,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -609,7 +607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -617,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -625,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -636,7 +634,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -644,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -652,7 +650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -660,7 +658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -668,7 +666,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -676,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -684,7 +682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -692,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -700,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -708,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -716,7 +714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -724,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -732,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -740,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -748,7 +746,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -756,7 +754,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -764,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -772,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -780,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -788,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -796,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -804,15 +802,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>40844</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -820,7 +821,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -828,7 +829,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -836,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -844,7 +845,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -852,7 +853,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -860,7 +861,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -868,7 +869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -876,7 +877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -884,7 +885,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
@@ -892,10 +893,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="2">
-        <v>40836</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
@@ -906,7 +907,7 @@
         <v>40836</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
         <v>37</v>
       </c>
@@ -914,7 +915,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
         <v>38</v>
       </c>
@@ -922,7 +923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
         <v>39</v>
       </c>
@@ -933,7 +934,7 @@
         <v>40838</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="3" t="s">
         <v>46</v>
       </c>
@@ -941,7 +942,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
         <v>48</v>
       </c>
@@ -956,24 +957,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Users can now print individual photo or an entire album. Also any user can run the cleanup script that will remove photos that no one is referencing in their albums. Updated requirements sheet too.
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="19155" windowHeight="8505"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -174,8 +174,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,6 +340,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -374,6 +375,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -549,21 +551,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -577,7 +579,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -591,7 +593,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -599,7 +601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -607,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -615,7 +617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -623,7 +625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -634,7 +636,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -642,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -650,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -658,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -666,7 +668,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -674,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -682,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -690,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -698,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -706,7 +708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -714,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -722,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -730,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -738,215 +740,205 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>40848</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>40844</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>30</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2">
-        <v>40844</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>21</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="6" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>40843</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2">
+        <v>40836</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2">
+        <v>40848</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2">
-        <v>40843</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="2">
-        <v>40836</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>39</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2">
+        <v>40838</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>46</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="2">
-        <v>40838</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -957,24 +949,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
switch user accounts now works fully. updated requirements sheet. fixed minor bugs
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -165,17 +165,41 @@
     <t>R-PR1</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>on remove album, removing last album and creating new one, recreates the new one and the one just removed. Check on close function for album</t>
+    <t>Right click add picture to different album</t>
+  </si>
+  <si>
+    <t>Allow user to search for phot names</t>
+  </si>
+  <si>
+    <t>Sort photos by criteria</t>
+  </si>
+  <si>
+    <t>Display timestamp of added photos and modified</t>
+  </si>
+  <si>
+    <t>Display resolution</t>
+  </si>
+  <si>
+    <t>Golden Rectangle</t>
+  </si>
+  <si>
+    <t>Confusion - ask cavan/john</t>
+  </si>
+  <si>
+    <t>The End-user shall have the option to view the photos within the album as a slideshow</t>
+  </si>
+  <si>
+    <t>Step forward/backward</t>
+  </si>
+  <si>
+    <t>Picture viewer will display caption displaying the photo’s name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +243,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -240,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -251,6 +281,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,9 +606,7 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -589,16 +618,16 @@
       <c r="C2" s="2">
         <v>40843</v>
       </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>40</v>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>40848</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -667,6 +696,9 @@
       <c r="B11" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -708,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -716,7 +748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -724,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -732,7 +764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -740,7 +772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -748,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -756,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -764,7 +796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -772,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -780,7 +812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -791,7 +823,7 @@
         <v>40848</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -802,23 +834,29 @@
         <v>40844</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -826,31 +864,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -858,23 +905,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>45</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
@@ -885,7 +938,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -896,7 +949,7 @@
         <v>40836</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
@@ -907,15 +960,18 @@
         <v>40848</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
@@ -926,7 +982,7 @@
         <v>40838</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>46</v>
       </c>
@@ -934,12 +990,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>40</v>
+      </c>
+      <c r="E43" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pictures now store the timestamp of when they were added and the last time they were modified.
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -586,7 +586,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,8 +879,8 @@
       <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>40</v>
+      <c r="B32" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="E32" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Checked for total # of image rotations so we do not prompt user to save an image when back to original state. Limited username and album name length 100 or characters or less. Minor bug fixes.
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -192,7 +192,7 @@
     <t>Step forward/backward</t>
   </si>
   <si>
-    <t>Picture viewer will display caption displaying the photo’s name</t>
+    <t>Picture viewer will display label displaying the photo’s name</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,8 +693,11 @@
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>40</v>
+      <c r="B11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>40849</v>
       </c>
       <c r="E11" t="s">
         <v>49</v>
@@ -863,13 +866,16 @@
       <c r="B30" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="C30" s="2">
+        <v>40850</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>40</v>
+      <c r="B31" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="E31" t="s">
         <v>57</v>
@@ -909,8 +915,11 @@
       <c r="A35" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>3</v>
+      <c r="B35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2">
+        <v>40850</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>58</v>
@@ -920,8 +929,11 @@
       <c r="A36" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>40</v>
+      <c r="B36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2">
+        <v>40850</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Photo viewer now displays resolution, date added, and date modified.
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>R-AC1</t>
@@ -199,7 +196,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,13 +222,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -278,10 +268,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,7 +575,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +587,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -610,7 +599,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -621,7 +610,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>1</v>
@@ -632,7 +621,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>1</v>
@@ -640,7 +629,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>1</v>
@@ -648,7 +637,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>1</v>
@@ -656,7 +645,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>1</v>
@@ -667,7 +656,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>1</v>
@@ -675,7 +664,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>1</v>
@@ -683,7 +672,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>1</v>
@@ -691,7 +680,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>1</v>
@@ -700,12 +689,12 @@
         <v>40849</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>1</v>
@@ -713,7 +702,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>1</v>
@@ -721,7 +710,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>1</v>
@@ -729,7 +718,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>1</v>
@@ -737,7 +726,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>1</v>
@@ -745,7 +734,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>1</v>
@@ -753,7 +742,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>1</v>
@@ -761,7 +750,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>1</v>
@@ -769,7 +758,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>1</v>
@@ -777,7 +766,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>1</v>
@@ -785,7 +774,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>1</v>
@@ -793,7 +782,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>1</v>
@@ -801,7 +790,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>1</v>
@@ -809,7 +798,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>1</v>
@@ -817,7 +806,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>1</v>
@@ -828,7 +817,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>1</v>
@@ -839,29 +828,29 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>40</v>
+        <v>19</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="E29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>1</v>
@@ -872,40 +861,46 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>3</v>
+        <v>27</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <v>40850</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>40</v>
+        <v>28</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <v>40850</v>
       </c>
       <c r="E33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>1</v>
@@ -913,7 +908,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>1</v>
@@ -921,13 +916,13 @@
       <c r="C35" s="2">
         <v>40850</v>
       </c>
-      <c r="E35" s="8" t="s">
-        <v>58</v>
+      <c r="E35" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>1</v>
@@ -935,13 +930,13 @@
       <c r="C36" s="2">
         <v>40850</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>56</v>
+      <c r="E36" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>1</v>
@@ -952,7 +947,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>1</v>
@@ -963,7 +958,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>1</v>
@@ -974,18 +969,18 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>1</v>
@@ -996,21 +991,21 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="E43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added search for photo by name capability, started fixing populate panel with thumbnails.
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Display resolution</t>
   </si>
   <si>
-    <t>Golden Rectangle</t>
-  </si>
-  <si>
     <t>Confusion - ask cavan/john</t>
   </si>
   <si>
@@ -190,13 +187,19 @@
   </si>
   <si>
     <t>Picture viewer will display label displaying the photo’s name</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Golden Rectangle, main form is correct size (approximately) but not resizeable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +242,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -260,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -271,6 +281,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +586,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,8 +841,8 @@
       <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>39</v>
+      <c r="B28" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="E28" t="s">
         <v>49</v>
@@ -867,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -917,7 +928,7 @@
         <v>40850</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -931,7 +942,7 @@
         <v>40850</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -971,11 +982,11 @@
       <c r="A40" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>39</v>
+      <c r="B40" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1005,7 +1016,7 @@
         <v>39</v>
       </c>
       <c r="E43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Disabled the photobox on image load now. Display a message that pictures are loading...
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="19155" windowHeight="8505"/>
@@ -165,9 +165,6 @@
     <t>Right click add picture to different album</t>
   </si>
   <si>
-    <t>Allow user to search for phot names</t>
-  </si>
-  <si>
     <t>Sort photos by criteria</t>
   </si>
   <si>
@@ -193,13 +190,16 @@
   </si>
   <si>
     <t>Golden Rectangle, main form is correct size (approximately) but not resizeable</t>
+  </si>
+  <si>
+    <t>Allow user to search for photo names</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,7 +371,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -406,7 +405,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -582,21 +580,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -608,7 +606,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -619,7 +617,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -630,7 +628,7 @@
         <v>40848</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -638,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -646,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -654,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -665,7 +663,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -673,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -681,7 +679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -689,7 +687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -703,7 +701,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -711,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -719,7 +717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -727,7 +725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -735,7 +733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -743,7 +741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -751,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -759,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -767,7 +765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -775,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -783,7 +781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -791,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -799,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -807,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -815,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -826,7 +824,7 @@
         <v>40848</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -837,18 +835,18 @@
         <v>40844</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -856,10 +854,10 @@
         <v>39</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -870,7 +868,7 @@
         <v>40850</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -878,10 +876,10 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -892,10 +890,10 @@
         <v>40850</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -906,10 +904,10 @@
         <v>40850</v>
       </c>
       <c r="E33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -917,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -928,10 +926,10 @@
         <v>40850</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -942,10 +940,10 @@
         <v>40850</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
@@ -956,7 +954,7 @@
         <v>40843</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="3" t="s">
         <v>35</v>
       </c>
@@ -967,7 +965,7 @@
         <v>40836</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
@@ -978,18 +976,18 @@
         <v>40848</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B40" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" t="s">
         <v>57</v>
       </c>
-      <c r="E40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="3" t="s">
         <v>38</v>
       </c>
@@ -1000,7 +998,7 @@
         <v>40838</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="3" t="s">
         <v>45</v>
       </c>
@@ -1008,7 +1006,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
@@ -1016,7 +1014,7 @@
         <v>39</v>
       </c>
       <c r="E43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1026,24 +1024,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ask user for confirmation on rotation of a GIF file save and informs them the rotation will not be saved. Also fixed bug of hitting the X in create/rename album dialog that would still rename the dialog.
</commit_message>
<xml_diff>
--- a/docs/requirements.xlsx
+++ b/docs/requirements.xlsx
@@ -584,7 +584,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -839,8 +839,11 @@
       <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>56</v>
+      <c r="B28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>40853</v>
       </c>
       <c r="E28" t="s">
         <v>58</v>
@@ -850,8 +853,11 @@
       <c r="A29" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>39</v>
+      <c r="B29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>40853</v>
       </c>
       <c r="E29" t="s">
         <v>49</v>
@@ -874,6 +880,9 @@
       </c>
       <c r="B31" s="4" t="s">
         <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>40850</v>
       </c>
       <c r="E31" t="s">
         <v>54</v>

</xml_diff>